<commit_message>
Atualizando base de dados da pesquisa via Streamlit
</commit_message>
<xml_diff>
--- a/base_dados_pesquisa_PO.xlsx
+++ b/base_dados_pesquisa_PO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,32 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ingrid.matos@mrv.com.br</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bizagi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ferramenta de Planejamento</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Muito importante.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>